<commit_message>
final improvement according to Tom's point
</commit_message>
<xml_diff>
--- a/graph/Record on hased code.xlsx
+++ b/graph/Record on hased code.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yil1/p2p-model-bondora/graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EEAD1D-AF19-EB4E-9BB9-F4D011610C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510BB9A4-AF7B-3046-A03B-A8194DF310DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15520" activeTab="1" xr2:uid="{2ABABA23-CFAA-B647-9CFE-BF0AB0A6408B}"/>
+    <workbookView xWindow="-17440" yWindow="-24740" windowWidth="37700" windowHeight="23380" activeTab="1" xr2:uid="{2ABABA23-CFAA-B647-9CFE-BF0AB0A6408B}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Improvement" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="59">
   <si>
     <t>Calrify: For 4 exclude list, we parallelly run the models. The comparision among 4 groups has no effect on model training, feature selection and hyperparameter tuning.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -174,6 +174,67 @@
   <si>
     <t>151568ddc12bea2d4fa97fe8f254a3408a7c88cfd8090ceb1ed1e990c07576bb</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'alpha': 0.2, 'lambda': 0.0001}</t>
+  </si>
+  <si>
+    <t>5a8ebf203943cb97f92ab6f4f641e9e7a2303ef40e9c95fc75d63759ab2306e1</t>
+  </si>
+  <si>
+    <t>bc0ae29acf90d329fad705919260e009ddb64b7cc0c3b3cff4d42d76428286e3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eaa2e128effaa12a3dd05b4ce8516e2f928b4df72d1d6ea83cabd73cefc5f099</t>
+  </si>
+  <si>
+    <t>48fb5634f5eb4175d9a16062d075bbbb454a97ef2560d0ac5e13b6264064464b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c4ce3cee3723654bef090339dea65e11487c1d5e62170b03af9a4ce86b1e7b89</t>
+  </si>
+  <si>
+    <t>f3dc6363a41c926cbe19cb8a5b5d1fe8798bf6bcedaa01c51ce7dce283e98d68</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'hidden': [200, 200], 'epochs': 10}</t>
+  </si>
+  <si>
+    <t>82b4a1e0ff5ef657a0b164b4ef71b7953f40b52aeb845c0d0890cf105b5ff802</t>
+  </si>
+  <si>
+    <t>9896077936c2887aa745130c41268a5b0ba19e0e94e02e944af736f0db27132f</t>
+  </si>
+  <si>
+    <t>4da6237525c1316caf06200bec8cc35fc3fb94b703b2481eb0735b8bc17884cd</t>
+  </si>
+  <si>
+    <t>6201ece752c95cbca7fdf29e8b0d46e9e7822cf0970319a4910b6882272c8762</t>
+  </si>
+  <si>
+    <t>45f37b0b61cc6af2e712ecd794968334320eec5fde6950cf7c9bc1ca37f871ce</t>
+  </si>
+  <si>
+    <t>11a4c2f8c3a7f3b8176196e39860d329574569ff5310a3257721fd4694e9ac13</t>
+  </si>
+  <si>
+    <t>9cdf59b4ad433a59144fb30e6ad344140da627c4f66d04c027a90c837961acd3</t>
+  </si>
+  <si>
+    <t>f3359fc3af41dc092f7c7f94e381d98d85bb6ef73a72bf60f77f81301b1b5b00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ac5f75a5e0bd602588cb43790e92ed7969b2b319571f6ceabea4b3b4dc889d5d</t>
+  </si>
+  <si>
+    <t>0e9617fd69ddaf52a371c16c0e967b2f09c8dd750171af239ed780caa0bc652c</t>
+  </si>
+  <si>
+    <t>4e3bc768f8b5045e7aeb73f104c94d5e9ba18e55d29725286a0aece2ee8f697a</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552B5ACF-CFF4-8B45-8590-9D82D717631E}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="176" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1113,75 +1174,49 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>30</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="17" thickBot="1">
       <c r="A9" s="4"/>
@@ -1212,19 +1247,19 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1232,10 +1267,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>3</v>
@@ -1244,7 +1279,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" thickBot="1">
@@ -1255,17 +1290,17 @@
         <v>15</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1"/>
@@ -1290,75 +1325,49 @@
       <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="19">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>20</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="19">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>36</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="20" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>34</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="17" thickBot="1">
       <c r="A20" s="4"/>
@@ -1389,19 +1398,19 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="19">
@@ -1409,10 +1418,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>3</v>
@@ -1432,17 +1441,17 @@
         <v>15</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="19">

</xml_diff>